<commit_message>
Adiciona regra para apresentacao de valores zero como '-' e inclui linha remuneracao liquida
</commit_message>
<xml_diff>
--- a/espec002_remuneracao-servidores/static/formulario-detalhamento.xlsx
+++ b/espec002_remuneracao-servidores/static/formulario-detalhamento.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Mês/Ano</t>
   </si>
@@ -91,28 +91,19 @@
     <t>Outubro/2019</t>
   </si>
   <si>
-    <t>Vencimento Básico</t>
+    <t>Remuneração Líquida</t>
   </si>
   <si>
-    <t>Composição dos Jetons Empresas (R$)</t>
+    <t>-</t>
   </si>
   <si>
-    <t>Empresa 1</t>
+    <t>Composição da Remuneração (R$)</t>
   </si>
   <si>
-    <t>Empresa 2</t>
+    <t>Remuneração Bruta</t>
   </si>
   <si>
-    <t>Empresa 3</t>
-  </si>
-  <si>
-    <t>Vantagens (R$)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Composição da Remuneração </t>
-  </si>
-  <si>
-    <t>Descontos (R$)</t>
+    <t>Remuneração Básica</t>
   </si>
 </sst>
 </file>
@@ -122,7 +113,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -189,7 +180,23 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="11"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -589,7 +596,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -663,87 +670,100 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="justify"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -751,33 +771,6 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="17" fontId="5" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -801,6 +794,9 @@
     </xf>
     <xf numFmtId="17" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -809,6 +805,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFF7E1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -978,15 +979,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:colOff>753532</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>106892</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
+      <xdr:colOff>1001182</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>333375</xdr:rowOff>
+      <xdr:rowOff>354542</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1010,7 +1011,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7277100" y="257175"/>
+          <a:off x="7304615" y="276225"/>
           <a:ext cx="247650" cy="247650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2266,303 +2267,283 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J47"/>
+  <dimension ref="B1:I44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="3.42578125" customWidth="1"/>
     <col min="3" max="3" width="31.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="1.5703125" customWidth="1"/>
     <col min="6" max="6" width="36.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:10" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="58" t="s">
+    <row r="1" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:9" s="40" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="60"/>
-    </row>
-    <row r="3" spans="2:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="61" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="53"/>
+    </row>
+    <row r="3" spans="2:9" s="40" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="63"/>
-    </row>
-    <row r="4" spans="2:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="57"/>
-    </row>
-    <row r="5" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="33"/>
-      <c r="C5" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="30">
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="56"/>
+    </row>
+    <row r="4" spans="2:9" s="40" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
+    </row>
+    <row r="5" spans="2:9" s="39" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="38"/>
+      <c r="C5" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="36">
         <f>SUM(D6:D12)</f>
         <v>18100.68</v>
       </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="34">
+      <c r="E5" s="35"/>
+      <c r="F5" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="37">
         <f>SUM(G6:G9)</f>
         <v>4833.04</v>
       </c>
-      <c r="I5" s="32"/>
-    </row>
-    <row r="6" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="35"/>
+    </row>
+    <row r="6" spans="2:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="28"/>
       <c r="C6" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="27">
+        <v>27</v>
+      </c>
+      <c r="D6" s="31">
         <v>14811.42</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24" t="s">
+      <c r="E6" s="31"/>
+      <c r="F6" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="36">
+      <c r="G6" s="32">
         <v>1629.26</v>
       </c>
-      <c r="I6" s="32"/>
-    </row>
-    <row r="7" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="35"/>
+      <c r="I6" s="27"/>
+    </row>
+    <row r="7" spans="2:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="28"/>
       <c r="C7" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24" t="s">
+      <c r="D7" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="32">
         <v>3203.78</v>
       </c>
     </row>
-    <row r="8" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="35"/>
+    <row r="8" spans="2:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="28"/>
       <c r="C8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24" t="s">
+      <c r="D8" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="36"/>
-      <c r="I8" s="32"/>
-    </row>
-    <row r="9" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="35"/>
-      <c r="C9" s="42" t="s">
+      <c r="G8" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="27"/>
+    </row>
+    <row r="9" spans="2:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="28"/>
+      <c r="C9" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="32"/>
+    </row>
+    <row r="10" spans="2:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="29"/>
+      <c r="C10" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="32"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="2:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="29"/>
+      <c r="C11" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="32"/>
+      <c r="I11" s="27"/>
+    </row>
+    <row r="12" spans="2:9" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="28"/>
+      <c r="C12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D12" s="42">
         <v>3289.26</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="36"/>
-    </row>
-    <row r="10" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="41"/>
-      <c r="C10" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="51"/>
-      <c r="G10" s="36"/>
-      <c r="I10" s="32"/>
-    </row>
-    <row r="11" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="41"/>
-      <c r="C11" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="36"/>
-      <c r="I11" s="32"/>
-    </row>
-    <row r="12" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="35"/>
-      <c r="C12" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="36"/>
-    </row>
-    <row r="13" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="57"/>
-    </row>
-    <row r="14" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="41"/>
-      <c r="C14" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="43">
-        <v>0</v>
-      </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="37"/>
-    </row>
-    <row r="15" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="44"/>
-      <c r="C15" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="43">
-        <v>0</v>
-      </c>
-      <c r="E15" s="50"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="38"/>
-    </row>
-    <row r="16" spans="2:10" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="46"/>
-      <c r="C16" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="48">
-        <v>0</v>
-      </c>
-      <c r="E16" s="49"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
-      <c r="J16" s="52"/>
-    </row>
-    <row r="17" spans="2:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-    </row>
-    <row r="18" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-    </row>
-    <row r="19" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="32"/>
+    </row>
+    <row r="13" spans="2:9" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="68"/>
+      <c r="C13" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="47">
+        <f>D5-G5</f>
+        <v>13267.64</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+    </row>
+    <row r="15" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="2:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="25"/>
+    </row>
+    <row r="40" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="25"/>
+    </row>
+    <row r="41" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="25"/>
+    </row>
     <row r="42" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="27"/>
-    </row>
-    <row r="43" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="27"/>
-    </row>
-    <row r="44" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="27"/>
-    </row>
-    <row r="45" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-    </row>
-    <row r="46" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+    </row>
+    <row r="43" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B13:G13"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
+    <mergeCell ref="D13:E13"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
   <pageSetup scale="79" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2594,51 +2575,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
     </row>
     <row r="2" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="64" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="69" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="68" t="s">
+      <c r="O2" s="64" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="65"/>
+      <c r="B3" s="61"/>
       <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
@@ -2672,8 +2653,8 @@
       <c r="M3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="70"/>
-      <c r="O3" s="71"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="67"/>
     </row>
     <row r="4" spans="2:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="22" t="s">

</xml_diff>